<commit_message>
Modele logique corps sbm (#84)
* MAJ modèle logique corps

* Correction des erreurs dans le modèle logique 0b2684b478cc36fa1b25a4ac67a324c87868b2e9
</commit_message>
<xml_diff>
--- a/main/ig/StructureDefinition-fr-lm-accidents-transfusionnels.xlsx
+++ b/main/ig/StructureDefinition-fr-lm-accidents-transfusionnels.xlsx
@@ -57,7 +57,7 @@
     <t>Date</t>
   </si>
   <si>
-    <t>2026-01-09T15:21:06+00:00</t>
+    <t>2026-01-16T13:49:34+00:00</t>
   </si>
   <si>
     <t>Publisher</t>
@@ -81,7 +81,7 @@
     <t>Description</t>
   </si>
   <si>
-    <t>Entrée Accident transfusionnel</t>
+    <t>Accident transfusionnel</t>
   </si>
   <si>
     <t>Purpose</t>

</xml_diff>